<commit_message>
FEAT message press space to spawn
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A36F1C-5ED6-43B8-827C-B2A5548E5C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9617C3-7922-4295-BE7C-85B3CA195F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
   <si>
     <t>Joueur</t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>Quand plusieurs joueurs, bugs lié a entites enemy je pense</t>
+  </si>
+  <si>
+    <t>MAJ nb de player sur la map a l'accueil</t>
+  </si>
+  <si>
+    <t>pas pouvoir acceder si nb joueur plein</t>
   </si>
 </sst>
 </file>
@@ -768,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472F8FD-387E-4F62-A0B6-0155C88C2FF1}">
-  <dimension ref="B3:B20"/>
+  <dimension ref="B3:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,6 +844,16 @@
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT Display of nb of player log on a mp
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9617C3-7922-4295-BE7C-85B3CA195F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0ACBC8-DA77-4A20-9F58-2F795E77256E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -777,7 +777,7 @@
   <dimension ref="B3:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
FIX bug when 2 or more player on map
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0ACBC8-DA77-4A20-9F58-2F795E77256E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6BB9C7-26E6-4711-AB48-049D04F1D69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t>Joueur</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Des fois la touche espace descend la fenetre</t>
   </si>
   <si>
-    <t>Optimiser enemy entities</t>
-  </si>
-  <si>
     <t>Message ereur front si serveur pas dispo</t>
   </si>
   <si>
@@ -288,13 +285,13 @@
     <t>POV d'un joueur bug desfois (mouvement souris trop brusque ?)</t>
   </si>
   <si>
-    <t>Quand plusieurs joueurs, bugs lié a entites enemy je pense</t>
-  </si>
-  <si>
     <t>MAJ nb de player sur la map a l'accueil</t>
   </si>
   <si>
     <t>pas pouvoir acceder si nb joueur plein</t>
+  </si>
+  <si>
+    <t>Faille xss/autre securités</t>
   </si>
 </sst>
 </file>
@@ -774,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472F8FD-387E-4F62-A0B6-0155C88C2FF1}">
-  <dimension ref="B3:B23"/>
+  <dimension ref="B6:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,16 +783,6 @@
     <col min="3" max="3" width="77.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>86</v>
-      </c>
-    </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>80</v>
@@ -818,7 +805,7 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.3">
@@ -838,22 +825,27 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
When kill, death's life come back to 100
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6BB9C7-26E6-4711-AB48-049D04F1D69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A3A0D5-8F04-4BB7-8D0F-B1F93C1C7DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
   <si>
     <t>Joueur</t>
   </si>
@@ -258,24 +258,12 @@
     <t>Animation sur les skins (marcher, sauter, mort…)</t>
   </si>
   <si>
-    <t>Opti map builder</t>
-  </si>
-  <si>
     <t>optimiser le code en general</t>
   </si>
   <si>
-    <t>Desactiver le tire quand on est en haut</t>
-  </si>
-  <si>
     <t>Guncontroller voir la balle partir au tir</t>
   </si>
   <si>
-    <t>Recharger barre de vie quand mort</t>
-  </si>
-  <si>
-    <t>Des fois la touche espace descend la fenetre</t>
-  </si>
-  <si>
     <t>Message ereur front si serveur pas dispo</t>
   </si>
   <si>
@@ -292,6 +280,12 @@
   </si>
   <si>
     <t>Faille xss/autre securités</t>
+  </si>
+  <si>
+    <t>Balles a l'infinie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joueur enemie haut dessus de la box </t>
   </si>
 </sst>
 </file>
@@ -771,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472F8FD-387E-4F62-A0B6-0155C88C2FF1}">
-  <dimension ref="B6:B25"/>
+  <dimension ref="B2:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,6 +777,16 @@
     <col min="3" max="3" width="77.77734375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>80</v>
@@ -790,62 +794,42 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat / SEE THE BULLET WHEN SHOT
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975A2F6E-97B3-4711-BCF3-547DE14D3134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386CDCF8-4B87-46D9-8F13-333818DA9E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
   <si>
     <t>Joueur</t>
   </si>
@@ -261,9 +261,6 @@
     <t>optimiser le code en general</t>
   </si>
   <si>
-    <t>Guncontroller voir la balle partir au tir</t>
-  </si>
-  <si>
     <t>Message ereur front si serveur pas dispo</t>
   </si>
   <si>
@@ -286,6 +283,12 @@
   </si>
   <si>
     <t>chat recharge la page</t>
+  </si>
+  <si>
+    <t>Comprendre pq update function don't works for enemy entites</t>
+  </si>
+  <si>
+    <t>Clique gauche viser</t>
   </si>
 </sst>
 </file>
@@ -366,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -392,6 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472F8FD-387E-4F62-A0B6-0155C88C2FF1}">
-  <dimension ref="B2:B21"/>
+  <dimension ref="B2:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,58 +782,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B2" s="11"/>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>80</v>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>85</v>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Save KD players; Add particles to presentation component;
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9245BAB-E8CB-4D26-A861-ECE1C5432373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FAB598A-C9FD-4E7E-8271-6BC96DBA7882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="Sources" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -756,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472F8FD-387E-4F62-A0B6-0155C88C2FF1}">
-  <dimension ref="B2:B20"/>
+  <dimension ref="B2:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,13 +799,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Presnetation and Particles OK
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FAB598A-C9FD-4E7E-8271-6BC96DBA7882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E3575D-8312-43FE-B35B-5F8AE8C86320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <sheet name="Sources" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -760,7 +759,7 @@
   <dimension ref="B2:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -774,6 +773,11 @@
         <v>79</v>
       </c>
     </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>75</v>
@@ -787,11 +791,6 @@
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Choix du skin OK; autre modif : opti ??
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404C68AA-4E73-43DA-8481-623AF69FD17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5B2C05-1D7D-4C0D-B5D8-3436B653E198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
   <si>
     <t>Joueur</t>
   </si>
@@ -255,9 +255,6 @@
     <t>Mini map ?</t>
   </si>
   <si>
-    <t>Animation sur les skins (marcher, sauter, mort…)</t>
-  </si>
-  <si>
     <t>optimiser le code en general</t>
   </si>
   <si>
@@ -270,13 +267,28 @@
     <t xml:space="preserve">joueur enemie haut dessus de la box </t>
   </si>
   <si>
-    <t>Comprendre pq update function don't works for enemy entites</t>
-  </si>
-  <si>
-    <t>Choix skin au début, pour differencier</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sauvegarder kd par joueurs ? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.8 environ de trop en z, psq skin est sur la box de detection </t>
+  </si>
+  <si>
+    <t>Animation perso (marcher, sauter, mort…)</t>
+  </si>
+  <si>
+    <t>Entity enemi : RegisterHandler_ for hit, death…</t>
+  </si>
+  <si>
+    <t>deleteRemotePlayer : enlever le perso de la scene</t>
+  </si>
+  <si>
+    <t>pour les différentes animatiosn. Mais la fonction qui envoie des msg entre les composant a pas l'air de marcher de fou</t>
+  </si>
+  <si>
+    <t>pour une prochiane co, sauvegarder dans le temps</t>
+  </si>
+  <si>
+    <t>afficher pseudo sur skins</t>
   </si>
 </sst>
 </file>
@@ -756,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472F8FD-387E-4F62-A0B6-0155C88C2FF1}">
-  <dimension ref="B2:B16"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,44 +780,58 @@
     <col min="3" max="3" width="77.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit Presentation vue and Particles
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5084B94B-9B31-4D7E-9798-AE5C45D89985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D53390-99D5-4BE6-AF49-2F59D247B3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22350" yWindow="1755" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pour la prochaine fois" sheetId="4" r:id="rId1"/>
@@ -270,9 +270,6 @@
     <t xml:space="preserve">Sauvegarder kd par joueurs ? </t>
   </si>
   <si>
-    <t xml:space="preserve">2.8 environ de trop en z, psq skin est sur la box de detection </t>
-  </si>
-  <si>
     <t>Animation perso (marcher, sauter, mort…)</t>
   </si>
   <si>
@@ -292,6 +289,9 @@
   </si>
   <si>
     <t>back/utils/spcler : connection =&gt; prend le dernier user : faire avec pseudo</t>
+  </si>
+  <si>
+    <t>2.8 environ de trop en z, psq skin est sur la box de detection ?</t>
   </si>
 </sst>
 </file>
@@ -774,7 +774,7 @@
   <dimension ref="B2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,35 +788,35 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
@@ -829,7 +829,7 @@
         <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
@@ -852,7 +852,7 @@
   <dimension ref="B2:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -965,7 +965,7 @@
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="3" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Enemy on the floor OK, but not hitbox. Animation when idle, walk, on hit OK. On death, move player to spawn so don't need this animation
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D53390-99D5-4BE6-AF49-2F59D247B3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB6B419-61CD-4817-AD8D-06DE1514A2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
   <si>
     <t>Joueur</t>
   </si>
@@ -264,34 +264,25 @@
     <t>Faille xss/autre securités</t>
   </si>
   <si>
-    <t xml:space="preserve">joueur enemie haut dessus de la box </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sauvegarder kd par joueurs ? </t>
   </si>
   <si>
-    <t>Animation perso (marcher, sauter, mort…)</t>
-  </si>
-  <si>
-    <t>Entity enemi : RegisterHandler_ for hit, death…</t>
-  </si>
-  <si>
     <t>deleteRemotePlayer : enlever le perso de la scene</t>
   </si>
   <si>
-    <t>pour les différentes animatiosn. Mais la fonction qui envoie des msg entre les composant a pas l'air de marcher de fou</t>
-  </si>
-  <si>
     <t>pour une prochiane co, sauvegarder dans le temps</t>
   </si>
   <si>
     <t>afficher pseudo sur skins</t>
   </si>
   <si>
-    <t>back/utils/spcler : connection =&gt; prend le dernier user : faire avec pseudo</t>
-  </si>
-  <si>
-    <t>2.8 environ de trop en z, psq skin est sur la box de detection ?</t>
+    <t>Joueur enemi sur le sol OK, mais hit box tjrs en l'air</t>
+  </si>
+  <si>
+    <t>pb : si on la baisse, elle bug avec le sol et tous les joueurs bug (kinematic controler)</t>
+  </si>
+  <si>
+    <t>back/utils/socket : connection =&gt; prend le dernier user : faire avec pseudo</t>
   </si>
 </sst>
 </file>
@@ -771,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472F8FD-387E-4F62-A0B6-0155C88C2FF1}">
-  <dimension ref="B2:C18"/>
+  <dimension ref="B3:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,62 +774,49 @@
     <col min="3" max="3" width="77.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>78</v>
       </c>
-      <c r="C2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit avant test : apparition bug
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB6B419-61CD-4817-AD8D-06DE1514A2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15E741C-5FEC-443D-A09F-7D098B889404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
   <si>
     <t>Joueur</t>
   </si>
@@ -283,13 +283,19 @@
   </si>
   <si>
     <t>back/utils/socket : connection =&gt; prend le dernier user : faire avec pseudo</t>
+  </si>
+  <si>
+    <t>checkMovement_</t>
+  </si>
+  <si>
+    <t>Ok pour déplacment en x, faire z, puis saut en y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +323,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="6">
@@ -363,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -387,6 +399,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -765,7 +780,7 @@
   <dimension ref="B3:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,6 +795,14 @@
       </c>
       <c r="C3" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Before add pseudo on player
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE9E789-FDBE-4C8F-9929-04F8B942F01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80686526-AB11-4FBD-BF96-BE6BE54D6117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -792,7 +792,7 @@
   <dimension ref="B3:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Auto delete chat. Clean project components
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EDC172-6E06-4C85-96F6-A561DBE98703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D66748-F1BF-426C-9A45-30644B3CF0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -291,13 +291,13 @@
     <t>Amélioration de la hitbox : quand un enemie regarde en bas ou en haut, la hitbox reste droite</t>
   </si>
   <si>
-    <t>Rotation des enemies : en haut/bas ? Tout le skin pivote c pas fou</t>
-  </si>
-  <si>
-    <t>Chat : timer pour supprimer les mg au fur et a meusure</t>
-  </si>
-  <si>
     <t>github projet/action</t>
+  </si>
+  <si>
+    <t>Rotation des enemies : en haut/bas ? Tout le skin se penche, c pas fou</t>
+  </si>
+  <si>
+    <t>&lt;- OUI OUI OUI  -^</t>
   </si>
 </sst>
 </file>
@@ -789,7 +789,7 @@
   <dimension ref="B3:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,7 +808,10 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
@@ -829,11 +832,6 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>76</v>
@@ -862,7 +860,7 @@
         <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Hitbox Okokok. Quand un perso se penche, le skin ne se penche, et donc la hitbox reste sur le skin
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D66748-F1BF-426C-9A45-30644B3CF0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EABCB8-EF00-4C10-8649-4F84AD79A5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
   <si>
     <t>Joueur</t>
   </si>
@@ -270,41 +270,32 @@
     <t>deleteRemotePlayer : enlever le perso de la scene</t>
   </si>
   <si>
-    <t>pour une prochiane co, sauvegarder dans le temps</t>
-  </si>
-  <si>
     <t>back/utils/socket : connection =&gt; prend le dernier user : faire avec pseudo</t>
   </si>
   <si>
-    <t xml:space="preserve">github pipeline ? </t>
-  </si>
-  <si>
-    <t>quand on tue quelqu’un, deplacer le perso au spawn</t>
-  </si>
-  <si>
     <t>fait pour le joueur, mais si il bouge pas ça modife pas sa position pour les aurtes joeuurs</t>
   </si>
   <si>
-    <t>Faire en sorte de pas pivoter tout le joueur quand il regarde en haut/bas ?</t>
-  </si>
-  <si>
-    <t>Amélioration de la hitbox : quand un enemie regarde en bas ou en haut, la hitbox reste droite</t>
-  </si>
-  <si>
-    <t>github projet/action</t>
-  </si>
-  <si>
-    <t>Rotation des enemies : en haut/bas ? Tout le skin se penche, c pas fou</t>
-  </si>
-  <si>
-    <t>&lt;- OUI OUI OUI  -^</t>
+    <t>pour une prochiane co, sauvegarder dans le temps ? Donc pouvoir se co avec un pseduo déjà enregistrée, mais pas connecté</t>
+  </si>
+  <si>
+    <t>faire en sorte que le site est accessible avec le www.</t>
+  </si>
+  <si>
+    <t>quand on tue quelqu’un, deplacer le perso au spawn, reglé ???</t>
+  </si>
+  <si>
+    <t>Faire en sorte que on peut pas jouer avec un pseudo, seulement si il est dans la game</t>
+  </si>
+  <si>
+    <t>pseduo taille max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,12 +323,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="6">
@@ -384,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -408,9 +393,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -786,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472F8FD-387E-4F62-A0B6-0155C88C2FF1}">
-  <dimension ref="B3:C23"/>
+  <dimension ref="B2:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,77 +780,65 @@
     <col min="3" max="3" width="77.77734375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="11"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delete remote player OK
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3662C54A-5820-4A4A-A5B1-A352A39AE89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFD620C-3132-4E5E-A0CB-216E282AF1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
   <si>
     <t>Joueur</t>
   </si>
@@ -265,9 +265,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sauvegarder kd par joueurs ? </t>
-  </si>
-  <si>
-    <t>deleteRemotePlayer : enlever le perso de la scene</t>
   </si>
   <si>
     <t>back/utils/socket : connection =&gt; prend le dernier user : faire avec pseudo</t>
@@ -765,9 +762,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472F8FD-387E-4F62-A0B6-0155C88C2FF1}">
-  <dimension ref="B2:C19"/>
+  <dimension ref="B3:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -775,11 +774,6 @@
     <col min="3" max="3" width="77.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-    </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
@@ -787,7 +781,12 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
@@ -800,7 +799,7 @@
         <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
@@ -815,20 +814,15 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backend : creation nouvel user avec ses infos, pas en récupérant le dernier log. Front login : récupération pseduo et skin, si déjà joué avant, et set dans variables. Bloquage connexion uniquement si meme pseudo dans la game
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFD620C-3132-4E5E-A0CB-216E282AF1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979D342B-3742-42C3-B3A9-C14E5B963303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
   <si>
     <t>Joueur</t>
   </si>
@@ -264,25 +264,16 @@
     <t>Faille xss/autre securités</t>
   </si>
   <si>
-    <t xml:space="preserve">Sauvegarder kd par joueurs ? </t>
-  </si>
-  <si>
-    <t>back/utils/socket : connection =&gt; prend le dernier user : faire avec pseudo</t>
-  </si>
-  <si>
     <t>fait pour le joueur, mais si il bouge pas ça modife pas sa position pour les aurtes joeuurs</t>
   </si>
   <si>
-    <t>pour une prochiane co, sauvegarder dans le temps ? Donc pouvoir se co avec un pseduo déjà enregistrée, mais pas connecté</t>
-  </si>
-  <si>
     <t>faire en sorte que le site est accessible avec le www.</t>
   </si>
   <si>
     <t>quand on tue quelqu’un, deplacer le perso au spawn, reglé ???</t>
   </si>
   <si>
-    <t>Faire en sorte que on peut pas jouer avec un pseudo, seulement si il est dans la game</t>
+    <t>Refaire page d'accueil</t>
   </si>
 </sst>
 </file>
@@ -765,7 +756,7 @@
   <dimension ref="B3:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -774,55 +765,42 @@
     <col min="3" max="3" width="77.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>75</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Amelioration Page présentation. Ajout map zombie, avec des rooms pour avoir 1 websocket qui gèrent les différentes maps
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF8A1E0-D93B-46F6-9DE9-2BCFBB46326A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB60BFC7-C77D-4308-A5F8-A47AEBCB9882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -246,10 +246,10 @@
     <t>quand on tue quelqu’un, deplacer le perso au spawn, reglé ???</t>
   </si>
   <si>
-    <t>Refaire page d'accueil</t>
-  </si>
-  <si>
     <t>Class : pompe, sniper, assault. Changer avec la molette</t>
+  </si>
+  <si>
+    <t>Testes de charge, pour voir cb de joueurs en même temps</t>
   </si>
 </sst>
 </file>
@@ -339,47 +339,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC65911"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC65911"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC65911"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC65911"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC65911"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -431,6 +391,14 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC65911"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -450,27 +418,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7915716-2713-41E1-9816-9CCA20688FB3}" name="Tableau1" displayName="Tableau1" ref="B2:D23" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7915716-2713-41E1-9816-9CCA20688FB3}" name="Tableau1" displayName="Tableau1" ref="B2:D23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="B2:D23" xr:uid="{E7915716-2713-41E1-9816-9CCA20688FB3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D23">
-    <sortCondition sortBy="cellColor" ref="C2:C23" dxfId="4"/>
+    <sortCondition sortBy="cellColor" ref="C2:C23" dxfId="9"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EA661427-8D94-457C-A65C-4EE1EBAD36E2}" name="Joueur" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{4394574E-E796-4468-AAC6-A974F3E14031}" name="Status" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{47977C51-0FB4-4F55-8C27-A36B14D5A6DE}" name="Description" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{EA661427-8D94-457C-A65C-4EE1EBAD36E2}" name="Joueur" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{4394574E-E796-4468-AAC6-A974F3E14031}" name="Status" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{47977C51-0FB4-4F55-8C27-A36B14D5A6DE}" name="Description" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{77AEF6EE-01D1-4A92-BFA0-29F81A708890}" name="Tableau2" displayName="Tableau2" ref="B26:D33" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{77AEF6EE-01D1-4A92-BFA0-29F81A708890}" name="Tableau2" displayName="Tableau2" ref="B26:D33" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="B26:D33" xr:uid="{77AEF6EE-01D1-4A92-BFA0-29F81A708890}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE90541C-012C-450D-AD18-D9593DD533FB}" name="Serveur" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{B844762E-CE41-4489-991E-1F9B51D54A32}" name="Status" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{47A6C676-2110-4B79-ABE2-52DA7A8D5E91}" name="Description" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{EE90541C-012C-450D-AD18-D9593DD533FB}" name="Serveur" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{B844762E-CE41-4489-991E-1F9B51D54A32}" name="Status" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{47A6C676-2110-4B79-ABE2-52DA7A8D5E91}" name="Description" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -481,7 +449,7 @@
   <autoFilter ref="B2:D22" xr:uid="{4F457B6A-00ED-4651-867B-FA9C08BB220E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{91F264E8-6982-49D2-B255-FE6350754B73}" name="US"/>
-    <tableColumn id="2" xr3:uid="{768D072E-2CFE-4653-8747-A37310AEDAA2}" name="Status" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{768D072E-2CFE-4653-8747-A37310AEDAA2}" name="Status" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{03F91A6C-7BE5-4FB8-9EAB-778C63862F1E}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -754,7 +722,7 @@
   <dimension ref="B5:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,9 +736,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>72</v>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
@@ -828,7 +796,7 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Affichage des skins en 3d. Ajout de skin pour le mode zombie. Upgrade ws to change client size when close
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB60BFC7-C77D-4308-A5F8-A47AEBCB9882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0F62B6-FD0A-4F39-92D5-00FFF503F6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>Joueur</t>
   </si>
@@ -105,12 +105,6 @@
     <t>Communication avec les fronts pour le multi (pos joueurs, tires…)</t>
   </si>
   <si>
-    <t>Pas déployer et giter les models non utilisés</t>
-  </si>
-  <si>
-    <t>Trier les models 3D</t>
-  </si>
-  <si>
     <t>List des personnes connectées</t>
   </si>
   <si>
@@ -210,9 +204,6 @@
     <t>Ensuite envoyer des données, et faire un système de stockage des dernière valeurs, et les renvoyer sur les gens de la socket</t>
   </si>
   <si>
-    <t>1 web socket par map, donc class pour générer, renvoie le /uri au front pour ses requetes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comment identifier un arrivant sur le websocket, savoir quand il est partie (requete toutes les 10s ?),  il récupère les données des autres. </t>
   </si>
   <si>
@@ -250,6 +241,12 @@
   </si>
   <si>
     <t>Testes de charge, pour voir cb de joueurs en même temps</t>
+  </si>
+  <si>
+    <t>En haut a droite changer de mode : solo/multi</t>
+  </si>
+  <si>
+    <t>solo = zombie</t>
   </si>
 </sst>
 </file>
@@ -286,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +302,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -318,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -335,11 +338,34 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC65911"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC65911"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -418,27 +444,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7915716-2713-41E1-9816-9CCA20688FB3}" name="Tableau1" displayName="Tableau1" ref="B2:D23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="B2:D23" xr:uid="{E7915716-2713-41E1-9816-9CCA20688FB3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D23">
-    <sortCondition sortBy="cellColor" ref="C2:C23" dxfId="9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7915716-2713-41E1-9816-9CCA20688FB3}" name="Tableau1" displayName="Tableau1" ref="B2:D25" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="B2:D25" xr:uid="{E7915716-2713-41E1-9816-9CCA20688FB3}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D25">
+    <sortCondition sortBy="cellColor" ref="C2:C25" dxfId="11"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EA661427-8D94-457C-A65C-4EE1EBAD36E2}" name="Joueur" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{4394574E-E796-4468-AAC6-A974F3E14031}" name="Status" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{47977C51-0FB4-4F55-8C27-A36B14D5A6DE}" name="Description" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{EA661427-8D94-457C-A65C-4EE1EBAD36E2}" name="Joueur" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{4394574E-E796-4468-AAC6-A974F3E14031}" name="Status" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{47977C51-0FB4-4F55-8C27-A36B14D5A6DE}" name="Description" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{77AEF6EE-01D1-4A92-BFA0-29F81A708890}" name="Tableau2" displayName="Tableau2" ref="B26:D33" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="B26:D33" xr:uid="{77AEF6EE-01D1-4A92-BFA0-29F81A708890}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{77AEF6EE-01D1-4A92-BFA0-29F81A708890}" name="Tableau2" displayName="Tableau2" ref="B28:D35" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B28:D35" xr:uid="{77AEF6EE-01D1-4A92-BFA0-29F81A708890}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE90541C-012C-450D-AD18-D9593DD533FB}" name="Serveur" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{B844762E-CE41-4489-991E-1F9B51D54A32}" name="Status" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{47A6C676-2110-4B79-ABE2-52DA7A8D5E91}" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{EE90541C-012C-450D-AD18-D9593DD533FB}" name="Serveur" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B844762E-CE41-4489-991E-1F9B51D54A32}" name="Status" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{47A6C676-2110-4B79-ABE2-52DA7A8D5E91}" name="Description" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -449,7 +475,7 @@
   <autoFilter ref="B2:D22" xr:uid="{4F457B6A-00ED-4651-867B-FA9C08BB220E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{91F264E8-6982-49D2-B255-FE6350754B73}" name="US"/>
-    <tableColumn id="2" xr3:uid="{768D072E-2CFE-4653-8747-A37310AEDAA2}" name="Status" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{768D072E-2CFE-4653-8747-A37310AEDAA2}" name="Status" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{03F91A6C-7BE5-4FB8-9EAB-778C63862F1E}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -719,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472F8FD-387E-4F62-A0B6-0155C88C2FF1}">
-  <dimension ref="B5:C13"/>
+  <dimension ref="B5:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,29 +759,50 @@
   <sheetData>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>69</v>
       </c>
     </row>
@@ -766,10 +813,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,13 +838,7 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="3" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
@@ -805,25 +846,15 @@
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="3"/>
     </row>
@@ -833,189 +864,199 @@
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C11" s="6"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C16" s="6"/>
-      <c r="D16" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C21" s="6"/>
-      <c r="D21" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C22" s="6"/>
-      <c r="D22" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="7"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D28" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-    </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1044,7 +1085,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -1055,20 +1096,20 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
@@ -1076,35 +1117,35 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9" s="5"/>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
@@ -1121,85 +1162,85 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1225,18 +1266,18 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Merge dev into main
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0F62B6-FD0A-4F39-92D5-00FFF503F6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF85955-9ABD-4D1C-86B9-D24C39BD883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
   <si>
     <t>Joueur</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>solo = zombie</t>
+  </si>
+  <si>
+    <t>VERIFIER LES POSITIONS DE SPAWN CARTE ZOMBIE</t>
+  </si>
+  <si>
+    <t>Si c les meme que space, on pourrait spanw a corte</t>
   </si>
 </sst>
 </file>
@@ -321,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -338,34 +344,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC65911"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC65911"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -444,27 +430,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7915716-2713-41E1-9816-9CCA20688FB3}" name="Tableau1" displayName="Tableau1" ref="B2:D25" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E7915716-2713-41E1-9816-9CCA20688FB3}" name="Tableau1" displayName="Tableau1" ref="B2:D25" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="B2:D25" xr:uid="{E7915716-2713-41E1-9816-9CCA20688FB3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D25">
-    <sortCondition sortBy="cellColor" ref="C2:C25" dxfId="11"/>
+    <sortCondition sortBy="cellColor" ref="C2:C25" dxfId="9"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EA661427-8D94-457C-A65C-4EE1EBAD36E2}" name="Joueur" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{4394574E-E796-4468-AAC6-A974F3E14031}" name="Status" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{47977C51-0FB4-4F55-8C27-A36B14D5A6DE}" name="Description" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{EA661427-8D94-457C-A65C-4EE1EBAD36E2}" name="Joueur" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{4394574E-E796-4468-AAC6-A974F3E14031}" name="Status" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{47977C51-0FB4-4F55-8C27-A36B14D5A6DE}" name="Description" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{77AEF6EE-01D1-4A92-BFA0-29F81A708890}" name="Tableau2" displayName="Tableau2" ref="B28:D35" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{77AEF6EE-01D1-4A92-BFA0-29F81A708890}" name="Tableau2" displayName="Tableau2" ref="B28:D35" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="B28:D35" xr:uid="{77AEF6EE-01D1-4A92-BFA0-29F81A708890}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE90541C-012C-450D-AD18-D9593DD533FB}" name="Serveur" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B844762E-CE41-4489-991E-1F9B51D54A32}" name="Status" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{47A6C676-2110-4B79-ABE2-52DA7A8D5E91}" name="Description" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{EE90541C-012C-450D-AD18-D9593DD533FB}" name="Serveur" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{B844762E-CE41-4489-991E-1F9B51D54A32}" name="Status" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{47A6C676-2110-4B79-ABE2-52DA7A8D5E91}" name="Description" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -475,7 +461,7 @@
   <autoFilter ref="B2:D22" xr:uid="{4F457B6A-00ED-4651-867B-FA9C08BB220E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{91F264E8-6982-49D2-B255-FE6350754B73}" name="US"/>
-    <tableColumn id="2" xr3:uid="{768D072E-2CFE-4653-8747-A37310AEDAA2}" name="Status" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{768D072E-2CFE-4653-8747-A37310AEDAA2}" name="Status" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{03F91A6C-7BE5-4FB8-9EAB-778C63862F1E}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -745,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472F8FD-387E-4F62-A0B6-0155C88C2FF1}">
-  <dimension ref="B5:C21"/>
+  <dimension ref="B3:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,6 +743,14 @@
     <col min="3" max="3" width="77.77734375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+    </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>64</v>
@@ -786,7 +780,7 @@
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C16" t="s">
@@ -794,15 +788,15 @@
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="8" t="s">
+      <c r="B19" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V1 READY ! Setup ping between client and server
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\WebFps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF85955-9ABD-4D1C-86B9-D24C39BD883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99820D47-D117-45B6-BE28-3A3FE2B0E0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Joueur</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Entrer un pseudo</t>
   </si>
   <si>
-    <t>Choisir classe pour les armes</t>
-  </si>
-  <si>
     <t>Afficher score</t>
   </si>
   <si>
@@ -228,18 +225,9 @@
     <t>Faille xss/autre securités</t>
   </si>
   <si>
-    <t>fait pour le joueur, mais si il bouge pas ça modife pas sa position pour les aurtes joeuurs</t>
-  </si>
-  <si>
     <t>faire en sorte que le site est accessible avec le www.</t>
   </si>
   <si>
-    <t>quand on tue quelqu’un, deplacer le perso au spawn, reglé ???</t>
-  </si>
-  <si>
-    <t>Class : pompe, sniper, assault. Changer avec la molette</t>
-  </si>
-  <si>
     <t>Testes de charge, pour voir cb de joueurs en même temps</t>
   </si>
   <si>
@@ -249,10 +237,10 @@
     <t>solo = zombie</t>
   </si>
   <si>
-    <t>VERIFIER LES POSITIONS DE SPAWN CARTE ZOMBIE</t>
-  </si>
-  <si>
-    <t>Si c les meme que space, on pourrait spanw a corte</t>
+    <t>Choix d'armes sous forme de class</t>
+  </si>
+  <si>
+    <t>assault, pompe, sniper…</t>
   </si>
 </sst>
 </file>
@@ -289,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,12 +296,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -327,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -344,7 +326,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -731,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472F8FD-387E-4F62-A0B6-0155C88C2FF1}">
-  <dimension ref="B3:C21"/>
+  <dimension ref="B3:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,61 +727,56 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>73</v>
+      <c r="B3" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>64</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>70</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" t="s">
-        <v>72</v>
-      </c>
-    </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>69</v>
-      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -825,10 +803,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
@@ -882,12 +860,12 @@
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="3"/>
@@ -901,7 +879,7 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
@@ -915,18 +893,18 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
@@ -938,7 +916,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
@@ -952,32 +930,32 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="3"/>
@@ -994,29 +972,29 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
@@ -1031,20 +1009,20 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
@@ -1079,31 +1057,31 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
@@ -1111,35 +1089,35 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9" s="5"/>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
@@ -1156,85 +1134,85 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1260,18 +1238,18 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>